<commit_message>
A Tudásteszt és a Szótár activityjének első változata, és módosítás az ütemtervben
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -355,18 +355,20 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,29 +501,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="C6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="F6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -709,6 +711,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -732,6 +737,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Új logóterv első, nem végleges változata
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -355,20 +355,20 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
@@ -712,7 +712,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -738,7 +738,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Módosítás az ütemterven (Gery részére)
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Funkció</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Szótár</t>
+  </si>
+  <si>
+    <t>Listakezelés</t>
+  </si>
+  <si>
+    <t>Lista elemeinek elgördíthetővé tétele, funkciók hozzáadása</t>
   </si>
   <si>
     <t>Adatbáziskezelés</t>
@@ -362,20 +368,20 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1275510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,7 +540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
@@ -545,74 +551,74 @@
         <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="n">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E9" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F9" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -623,76 +629,103 @@
         <v>1</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F11" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="0" t="n">
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F12" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
+      <c r="B13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -722,7 +755,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -748,7 +781,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Geryson Spinner megvalósításának behelyezése, WordUpdateObject fgv elkészítése (ezzel már több módosítást végre lehet hajtani egy rekordon, anélkül, hogy több vagy többször (kellene) függvényt hívnunk
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Funkció</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>elemi és bővített fgv.ek tesztelése (unittest segítségével)</t>
+  </si>
+  <si>
+    <t>Presenter fgv-ek</t>
+  </si>
+  <si>
+    <t>Word</t>
   </si>
 </sst>
 </file>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,13 +841,13 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -916,10 +922,10 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -939,13 +945,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -990,14 +996,14 @@
       <c r="D14">
         <v>15</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>29</v>
+      <c r="E14" s="9">
+        <v>20</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
         <v>20</v>
@@ -1005,38 +1011,56 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="E15" s="9"/>
       <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A18" r:id="rId1"/>
+    <hyperlink ref="A19" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Junit test, pár fgv dokumentálása
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Funkció</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Tesztelés</t>
   </si>
   <si>
-    <t>elemi és bővített fgv.ek tesztelése (unittest segítségével)</t>
-  </si>
-  <si>
     <t>Presenter fgv-ek</t>
   </si>
   <si>
@@ -135,6 +132,15 @@
   </si>
   <si>
     <t>Kezdő, betöltő animáció</t>
+  </si>
+  <si>
+    <t>elemi és bővített fgv.ek tesztelése</t>
+  </si>
+  <si>
+    <t>Esztétika</t>
+  </si>
+  <si>
+    <t>Osztályok szeparálása</t>
   </si>
 </sst>
 </file>
@@ -632,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +971,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
@@ -1017,10 +1023,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1038,7 +1044,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1050,10 +1056,10 @@
         <v>29</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>
@@ -1061,10 +1067,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1085,14 +1091,40 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A19" r:id="rId1"/>
+    <hyperlink ref="A27" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
LoggerMain.java létrehozása, loggoló fgv elkészítése
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Funkció</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>Osztályok szeparálása</t>
+  </si>
+  <si>
+    <t>Logger</t>
+  </si>
+  <si>
+    <t>osztály létrehozása, működtetése</t>
+  </si>
+  <si>
+    <t>Dokumentálás</t>
+  </si>
+  <si>
+    <t>adatbázis osztályok függvényeinek dokumentálása</t>
   </si>
 </sst>
 </file>
@@ -641,7 +653,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,10 +1068,10 @@
         <v>29</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>
@@ -1114,6 +1126,49 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Donate funkció beépítése Kicsit laggos lett az animáció
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Funkció</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>adatbázis osztályok függvényeinek dokumentálása</t>
+  </si>
+  <si>
+    <t>Donate</t>
+  </si>
+  <si>
+    <t>Paypal donate funkció beépítése webView segítségével</t>
   </si>
 </sst>
 </file>
@@ -653,7 +659,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,6 +1175,29 @@
         <v>2</v>
       </c>
       <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="H21" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Donate, internetkapcsolat ellenőrzésének beépítése
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Funkció</t>
   </si>
@@ -122,12 +122,6 @@
     <t>Tesztelés</t>
   </si>
   <si>
-    <t>Presenter fgv-ek</t>
-  </si>
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
     <t>Animáció</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Paypal donate funkció beépítése webView segítségével</t>
+  </si>
+  <si>
+    <t>Súgó</t>
+  </si>
+  <si>
+    <t>program alapadatai és leírása</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +214,20 @@
         <bgColor rgb="FF00CC00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0CA430"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -258,6 +270,152 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -265,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,16 +434,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -360,6 +541,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0CA430"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -656,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +859,7 @@
     <col min="9" max="1025" width="8.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,517 +885,531 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C2" s="29">
+        <v>2</v>
+      </c>
+      <c r="D2" s="29">
+        <v>2</v>
+      </c>
+      <c r="E2" s="29">
+        <v>1</v>
+      </c>
+      <c r="F2" s="29">
+        <v>2</v>
+      </c>
+      <c r="G2" s="29">
+        <v>1</v>
+      </c>
+      <c r="H2" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
         <v>4</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
         <v>0</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12">
         <v>3</v>
       </c>
-      <c r="F6" s="4">
-        <v>2</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="F6" s="12">
+        <v>2</v>
+      </c>
+      <c r="G6" s="12">
         <v>0</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="9">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="C8" s="15">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
+      <c r="E8" s="15">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="15">
         <v>7</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="15">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18">
         <v>8</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="18">
         <v>12</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="18">
         <v>12</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="18">
         <v>0</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="C10" s="15">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+      <c r="G10" s="15">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2</v>
+      </c>
+      <c r="E11" s="15">
         <v>8</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="15">
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="15">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
         <v>8</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="9">
         <v>15</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <v>14</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>15</v>
+      </c>
+      <c r="E14" s="23">
+        <v>20</v>
+      </c>
+      <c r="F14" s="9">
+        <v>16</v>
+      </c>
+      <c r="G14" s="9">
+        <v>4</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="9">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9">
+        <v>10</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="9">
+        <v>2</v>
+      </c>
+      <c r="G15" s="9">
+        <v>8</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
+      <c r="D16" s="15">
+        <v>4</v>
+      </c>
+      <c r="E16" s="15">
+        <v>5</v>
+      </c>
+      <c r="F16" s="15">
+        <v>5</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15">
+        <v>5</v>
+      </c>
+      <c r="F17" s="15">
+        <v>5</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
+      <c r="B18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9">
+        <v>4</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9">
+        <v>2</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="9">
         <v>3</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="D19" s="9">
+        <v>3</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="9">
+        <v>2</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="15">
+        <v>3</v>
+      </c>
+      <c r="D20" s="15">
+        <v>2</v>
+      </c>
+      <c r="E20" s="15">
+        <v>5</v>
+      </c>
+      <c r="F20" s="15">
+        <v>5</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="25">
+        <v>3</v>
+      </c>
+      <c r="D21" s="25">
+        <v>3</v>
+      </c>
+      <c r="E21" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F13">
+      <c r="F21" s="25">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="G21" s="25">
+        <v>3</v>
+      </c>
+      <c r="H21" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>15</v>
-      </c>
-      <c r="E14" s="9">
-        <v>20</v>
-      </c>
-      <c r="F14">
-        <v>16</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>8</v>
-      </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="H19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-      <c r="H21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A27" r:id="rId1"/>
+    <hyperlink ref="A26" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Loggolás a Database fgv-ekben
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -140,9 +140,6 @@
     <t>Logger</t>
   </si>
   <si>
-    <t>osztály létrehozása, működtetése</t>
-  </si>
-  <si>
     <t>Dokumentálás</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>program alapadatai és leírása</t>
+  </si>
+  <si>
+    <t>adatbázis fgv-ben loggolás</t>
   </si>
 </sst>
 </file>
@@ -210,12 +210,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0FA907"/>
-        <bgColor rgb="FF00CC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0CA430"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -226,6 +220,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0CA430"/>
+        <bgColor rgb="FF00CC00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -423,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,13 +444,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -458,15 +455,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -843,7 +847,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,28 +890,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29">
-        <v>2</v>
-      </c>
-      <c r="D2" s="29">
-        <v>2</v>
-      </c>
-      <c r="E2" s="29">
-        <v>1</v>
-      </c>
-      <c r="F2" s="29">
-        <v>2</v>
-      </c>
-      <c r="G2" s="29">
-        <v>1</v>
-      </c>
-      <c r="H2" s="30" t="s">
+      <c r="C2" s="26">
+        <v>2</v>
+      </c>
+      <c r="D2" s="26">
+        <v>2</v>
+      </c>
+      <c r="E2" s="26">
+        <v>1</v>
+      </c>
+      <c r="F2" s="26">
+        <v>2</v>
+      </c>
+      <c r="G2" s="26">
+        <v>1</v>
+      </c>
+      <c r="H2" s="27" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1068,33 +1072,33 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="18">
-        <v>1</v>
-      </c>
-      <c r="D9" s="18">
+      <c r="C9" s="31">
+        <v>1</v>
+      </c>
+      <c r="D9" s="31">
         <v>8</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="31">
         <v>12</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="31">
         <v>12</v>
       </c>
-      <c r="G9" s="18">
-        <v>0</v>
-      </c>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="31">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -1120,7 +1124,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -1146,33 +1150,33 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
         <v>8</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="15">
         <v>15</v>
       </c>
-      <c r="F12" s="9">
-        <v>14</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10" t="s">
+      <c r="F12" s="15">
+        <v>15</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1184,7 +1188,7 @@
       <c r="D13" s="9">
         <v>1</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="9">
@@ -1198,33 +1202,33 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="9">
-        <v>2</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="C14" s="15">
+        <v>2</v>
+      </c>
+      <c r="D14" s="15">
         <v>15</v>
       </c>
-      <c r="E14" s="23">
-        <v>20</v>
-      </c>
-      <c r="F14" s="9">
-        <v>16</v>
-      </c>
-      <c r="G14" s="9">
-        <v>4</v>
-      </c>
-      <c r="H14" s="10" t="s">
+      <c r="E14" s="28">
+        <v>20</v>
+      </c>
+      <c r="F14" s="15">
+        <v>20</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1236,7 +1240,7 @@
       <c r="D15" s="9">
         <v>10</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="9">
@@ -1250,7 +1254,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -1276,7 +1280,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -1302,57 +1306,63 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+      <c r="D18" s="15">
+        <v>4</v>
+      </c>
+      <c r="E18" s="15">
+        <v>3</v>
+      </c>
+      <c r="F18" s="15">
+        <v>3</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="9">
-        <v>2</v>
-      </c>
-      <c r="D18" s="9">
-        <v>4</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9">
-        <v>2</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="B19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="15">
+        <v>3</v>
+      </c>
+      <c r="D19" s="15">
+        <v>3</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="15">
+        <v>3</v>
+      </c>
+      <c r="G19" s="15">
+        <v>3</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9">
-        <v>3</v>
-      </c>
-      <c r="D19" s="9">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9">
-        <v>2</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="B20" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="C20" s="15">
         <v>3</v>
@@ -1374,30 +1384,33 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="25">
-        <v>3</v>
-      </c>
-      <c r="D21" s="25">
-        <v>3</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="25">
-        <v>0</v>
-      </c>
-      <c r="G21" s="25">
-        <v>3</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>20</v>
-      </c>
+      <c r="C21" s="22">
+        <v>3</v>
+      </c>
+      <c r="D21" s="22">
+        <v>3</v>
+      </c>
+      <c r="E21" s="23">
+        <v>5</v>
+      </c>
+      <c r="F21" s="22">
+        <v>1</v>
+      </c>
+      <c r="G21" s="22">
+        <v>4</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="29"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">

</xml_diff>

<commit_message>
Súgóba a learn videó működésre bírva, bár a mérettel nem vagyok kiegyezve, de ez a videó sajátosságából fakad - Ütemtervben a feladatok folyamatának aktualizálása - DescriptionActivity.java -ban az activity mérete normál méretűvé módosítása - videó hozzáadása a projekthez mint erőforrás
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Funkció</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>adatbázis fgv-ben loggolás</t>
+  </si>
+  <si>
+    <t>help videó beépítése</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,18 +452,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -471,6 +465,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -847,7 +847,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,28 +890,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26">
-        <v>2</v>
-      </c>
-      <c r="E2" s="26">
-        <v>1</v>
-      </c>
-      <c r="F2" s="26">
-        <v>2</v>
-      </c>
-      <c r="G2" s="26">
-        <v>1</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="21">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21">
+        <v>2</v>
+      </c>
+      <c r="E2" s="21">
+        <v>1</v>
+      </c>
+      <c r="F2" s="21">
+        <v>2</v>
+      </c>
+      <c r="G2" s="21">
+        <v>1</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1072,28 +1072,28 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="31">
-        <v>1</v>
-      </c>
-      <c r="D9" s="31">
+      <c r="C9" s="26">
+        <v>1</v>
+      </c>
+      <c r="D9" s="26">
         <v>8</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="26">
         <v>12</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="26">
         <v>12</v>
       </c>
-      <c r="G9" s="31">
-        <v>0</v>
-      </c>
-      <c r="H9" s="32" t="s">
+      <c r="G9" s="26">
+        <v>0</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1176,28 +1176,28 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="9">
-        <v>3</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19" t="s">
+      <c r="C13" s="15">
+        <v>3</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
-      <c r="H13" s="10" t="s">
+      <c r="F13" s="15">
+        <v>1</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
       <c r="D14" s="15">
         <v>15</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="23">
         <v>20</v>
       </c>
       <c r="F14" s="15">
@@ -1240,7 +1240,7 @@
       <c r="D15" s="9">
         <v>10</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="9">
@@ -1344,7 +1344,7 @@
       <c r="D19" s="15">
         <v>3</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="15">
@@ -1384,33 +1384,59 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="22">
-        <v>3</v>
-      </c>
-      <c r="D21" s="22">
-        <v>3</v>
+      <c r="C21" s="15">
+        <v>3</v>
+      </c>
+      <c r="D21" s="15">
+        <v>2</v>
       </c>
       <c r="E21" s="23">
-        <v>5</v>
-      </c>
-      <c r="F21" s="22">
-        <v>1</v>
-      </c>
-      <c r="G21" s="22">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="29">
         <v>4</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="D22" s="29">
+        <v>2</v>
+      </c>
+      <c r="E22" s="29">
+        <v>6</v>
+      </c>
+      <c r="F22" s="29">
+        <v>6</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0</v>
+      </c>
+      <c r="H22" s="30" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="29"/>
+      <c r="H23" s="24"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">

</xml_diff>

<commit_message>
Animáció elkészítve mely nem lett aktiválva - pontszám és eredmény a tudástesztbe
</commit_message>
<xml_diff>
--- a/program leírási dokumentációk/Ütemterv.xlsx
+++ b/program leírási dokumentációk/Ütemterv.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Funkció</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>help videó beépítése</t>
+  </si>
+  <si>
+    <t>A kezdő activity és a nyelvválasztás közötti animáció</t>
+  </si>
+  <si>
+    <t>Tudásteszt</t>
+  </si>
+  <si>
+    <t>hangjelzés beszúrása (sikeres megoldáskor megszólal)</t>
+  </si>
+  <si>
+    <t>kevesebb mint 1</t>
   </si>
 </sst>
 </file>
@@ -426,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -469,6 +481,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -844,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +874,7 @@
     <col min="2" max="2" width="53.28515625"/>
     <col min="3" max="3" width="8.140625"/>
     <col min="4" max="4" width="12.28515625"/>
-    <col min="5" max="5" width="14.28515625"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.85546875"/>
     <col min="7" max="7" width="18"/>
     <col min="8" max="8" width="11"/>
@@ -1280,49 +1298,49 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="15">
-        <v>3</v>
-      </c>
-      <c r="D17" s="15">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="A17" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="33">
+        <v>3</v>
+      </c>
+      <c r="D17" s="33">
         <v>5</v>
       </c>
-      <c r="F17" s="15">
+      <c r="E17" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
         <v>5</v>
       </c>
-      <c r="G17" s="15">
-        <v>0</v>
-      </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C18" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E18" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F18" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18" s="15">
         <v>0</v>
@@ -1333,25 +1351,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C19" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="15">
-        <v>3</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>29</v>
+        <v>4</v>
+      </c>
+      <c r="E19" s="15">
+        <v>3</v>
       </c>
       <c r="F19" s="15">
         <v>3</v>
       </c>
       <c r="G19" s="15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H19" s="16" t="s">
         <v>20</v>
@@ -1359,22 +1377,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C20" s="15">
         <v>3</v>
       </c>
       <c r="D20" s="15">
-        <v>2</v>
-      </c>
-      <c r="E20" s="15">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="F20" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G20" s="15">
         <v>0</v>
@@ -1385,67 +1403,119 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="15">
+        <v>3</v>
+      </c>
+      <c r="D21" s="15">
+        <v>3</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="15">
+        <v>3</v>
+      </c>
+      <c r="G21" s="15">
+        <v>3</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="15">
+        <v>3</v>
+      </c>
+      <c r="D22" s="15">
+        <v>2</v>
+      </c>
+      <c r="E22" s="15">
+        <v>5</v>
+      </c>
+      <c r="F22" s="15">
+        <v>5</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="15">
-        <v>3</v>
-      </c>
-      <c r="D21" s="15">
-        <v>2</v>
-      </c>
-      <c r="E21" s="23">
-        <v>1</v>
-      </c>
-      <c r="F21" s="15">
-        <v>1</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="C23" s="15">
+        <v>3</v>
+      </c>
+      <c r="D23" s="15">
+        <v>2</v>
+      </c>
+      <c r="E23" s="23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B24" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C24" s="29">
         <v>4</v>
       </c>
-      <c r="D22" s="29">
-        <v>2</v>
-      </c>
-      <c r="E22" s="29">
+      <c r="D24" s="29">
+        <v>2</v>
+      </c>
+      <c r="E24" s="29">
         <v>6</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F24" s="29">
         <v>6</v>
       </c>
-      <c r="G22" s="29">
-        <v>0</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="24"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="24"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A26" r:id="rId1"/>
+    <hyperlink ref="A28" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>

</xml_diff>